<commit_message>
retirado o sistema de data, alterado o aparecimento dos inputs de indicado
</commit_message>
<xml_diff>
--- a/dados/dados.xlsx
+++ b/dados/dados.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="dados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,58 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>jose brito</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>renault duster</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>tokio</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>225.00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>15/07/2024</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>16/07/2025</t>
+        </is>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionado sistema de formatação e verificação de datas, alterado tamanho da janela
</commit_message>
<xml_diff>
--- a/dados/dados.xlsx
+++ b/dados/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,47 +498,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>jose brito</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>renault duster</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>tokio</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>225.00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>6000</t>
-        </is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>111</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1500</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>15/07/2024</t>
+          <t>18/07/2024</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>16/07/2025</t>
+          <t>18/07/2025</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -546,6 +538,154 @@
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bbb</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>15</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2250</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>18/02/2024</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>18/02/2025</t>
+        </is>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>bbb</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>150</v>
+      </c>
+      <c r="G4" t="n">
+        <v>155</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>15/07/2004</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>15/07/2005</t>
+        </is>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hugo Rios Brito</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Porsche GT3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BRADESCO SEGUROS</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>20000</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2000.00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>3500</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>15/07/2004</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>15/07/2005</t>
+        </is>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>THEUREN</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Mudança na verificação de campos, e outras pequenas alterações
</commit_message>
<xml_diff>
--- a/dados/dados.xlsx
+++ b/dados/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,39 +498,41 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>carlos</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>carro legal</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>Tokio</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>111</v>
+        <v>1200</v>
       </c>
       <c r="E2" t="n">
         <v>10</v>
       </c>
-      <c r="F2" t="n">
-        <v>11.1</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>120.00</t>
+        </is>
       </c>
       <c r="G2" t="n">
         <v>1500</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>18/07/2024</t>
+          <t>15/07/2004</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>18/07/2025</t>
+          <t>15/07/2006</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -538,154 +540,6 @@
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>bbb</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>aaa</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>aaa</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>15000</v>
-      </c>
-      <c r="E3" t="n">
-        <v>15</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2250</v>
-      </c>
-      <c r="G3" t="n">
-        <v>5000</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>18/02/2024</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>18/02/2025</t>
-        </is>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ccc</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>bbb</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ccc</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1500</v>
-      </c>
-      <c r="E4" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" t="n">
-        <v>150</v>
-      </c>
-      <c r="G4" t="n">
-        <v>155</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>15/07/2004</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>15/07/2005</t>
-        </is>
-      </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hugo Rios Brito</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Porsche GT3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>BRADESCO SEGUROS</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>20000</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2000.00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>3500</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>15/07/2004</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>15/07/2005</t>
-        </is>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>THEUREN</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>